<commit_message>
Completed EDA entirely with new pipeline
</commit_message>
<xml_diff>
--- a/gpp-project/backend/vital_signs_comparison.xlsx
+++ b/gpp-project/backend/vital_signs_comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikhil\Downloads\SSN\College Files\Grand Project\RespirationHealth\gpp-project\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505FF937-BA50-4C3C-B60B-232B88694466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC9F146-D34E-4821-9CA2-A50999BE61E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5B8E4227-B513-4299-A02C-5553EB35DCD9}"/>
   </bookViews>
@@ -411,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F49D67A6-A7FB-4C09-9CF7-94A675027060}">
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G232"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+    <sheetView tabSelected="1" topLeftCell="A205" zoomScale="89" workbookViewId="0">
+      <selection activeCell="H218" sqref="H218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2889,6 +2889,2881 @@
         <v>91.97</v>
       </c>
     </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A108" s="2">
+        <v>107</v>
+      </c>
+      <c r="B108">
+        <v>9</v>
+      </c>
+      <c r="C108">
+        <v>55.99</v>
+      </c>
+      <c r="D108">
+        <v>8.11</v>
+      </c>
+      <c r="E108">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="F108">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G108">
+        <v>63.83</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A109" s="2">
+        <v>108</v>
+      </c>
+      <c r="B109">
+        <v>8</v>
+      </c>
+      <c r="C109">
+        <v>57.55</v>
+      </c>
+      <c r="D109">
+        <v>9.25</v>
+      </c>
+      <c r="E109">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="F109">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G109">
+        <v>65.61</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A110" s="2">
+        <v>109</v>
+      </c>
+      <c r="B110">
+        <v>10</v>
+      </c>
+      <c r="C110">
+        <v>55.46</v>
+      </c>
+      <c r="D110">
+        <v>8.23</v>
+      </c>
+      <c r="E110">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="F110">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G110">
+        <v>63.22</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A111" s="2">
+        <v>110</v>
+      </c>
+      <c r="B111">
+        <v>9</v>
+      </c>
+      <c r="C111">
+        <v>56.26</v>
+      </c>
+      <c r="D111">
+        <v>9.11</v>
+      </c>
+      <c r="E111">
+        <v>0.36</v>
+      </c>
+      <c r="F111">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G111">
+        <v>64.14</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A112" s="2">
+        <v>111</v>
+      </c>
+      <c r="B112">
+        <v>11</v>
+      </c>
+      <c r="C112">
+        <v>57.64</v>
+      </c>
+      <c r="D112">
+        <v>9.19</v>
+      </c>
+      <c r="E112">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="F112">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G112">
+        <v>65.709999999999994</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A113" s="2">
+        <v>112</v>
+      </c>
+      <c r="B113">
+        <v>8</v>
+      </c>
+      <c r="C113">
+        <v>54.97</v>
+      </c>
+      <c r="D113">
+        <v>8.74</v>
+      </c>
+      <c r="E113">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="F113">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G113">
+        <v>62.67</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A114" s="2">
+        <v>113</v>
+      </c>
+      <c r="B114">
+        <v>10</v>
+      </c>
+      <c r="C114">
+        <v>57.16</v>
+      </c>
+      <c r="D114">
+        <v>9.06</v>
+      </c>
+      <c r="E114">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="F114">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G114">
+        <v>65.16</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A115" s="2">
+        <v>114</v>
+      </c>
+      <c r="B115">
+        <v>9</v>
+      </c>
+      <c r="C115">
+        <v>55.14</v>
+      </c>
+      <c r="D115">
+        <v>9.18</v>
+      </c>
+      <c r="E115">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="F115">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G115">
+        <v>62.86</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A116" s="2">
+        <v>115</v>
+      </c>
+      <c r="B116">
+        <v>11</v>
+      </c>
+      <c r="C116">
+        <v>57.3</v>
+      </c>
+      <c r="D116">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="E116">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="F116">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G116">
+        <v>65.319999999999993</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A117" s="2">
+        <v>116</v>
+      </c>
+      <c r="B117">
+        <v>8</v>
+      </c>
+      <c r="C117">
+        <v>54.72</v>
+      </c>
+      <c r="D117">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="E117">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="F117">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G117">
+        <v>62.38</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A118" s="2">
+        <v>117</v>
+      </c>
+      <c r="B118">
+        <v>10</v>
+      </c>
+      <c r="C118">
+        <v>56.8</v>
+      </c>
+      <c r="D118">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="E118">
+        <v>0.36</v>
+      </c>
+      <c r="F118">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G118">
+        <v>64.75</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A119" s="2">
+        <v>118</v>
+      </c>
+      <c r="B119">
+        <v>9</v>
+      </c>
+      <c r="C119">
+        <v>54.92</v>
+      </c>
+      <c r="D119">
+        <v>8.36</v>
+      </c>
+      <c r="E119">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="F119">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G119">
+        <v>62.61</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A120" s="2">
+        <v>119</v>
+      </c>
+      <c r="B120">
+        <v>11</v>
+      </c>
+      <c r="C120">
+        <v>58.07</v>
+      </c>
+      <c r="D120">
+        <v>9.06</v>
+      </c>
+      <c r="E120">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="F120">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G120">
+        <v>66.2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A121" s="2">
+        <v>120</v>
+      </c>
+      <c r="B121">
+        <v>8</v>
+      </c>
+      <c r="C121">
+        <v>54.7</v>
+      </c>
+      <c r="D121">
+        <v>8.9700000000000006</v>
+      </c>
+      <c r="E121">
+        <v>0.34</v>
+      </c>
+      <c r="F121">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="G121">
+        <v>62.36</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A122" s="2">
+        <v>121</v>
+      </c>
+      <c r="B122">
+        <v>10</v>
+      </c>
+      <c r="C122">
+        <v>57.28</v>
+      </c>
+      <c r="D122">
+        <v>9.18</v>
+      </c>
+      <c r="E122">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="F122">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G122">
+        <v>65.3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A123" s="2">
+        <v>122</v>
+      </c>
+      <c r="B123">
+        <v>9</v>
+      </c>
+      <c r="C123">
+        <v>54.73</v>
+      </c>
+      <c r="D123">
+        <v>9.07</v>
+      </c>
+      <c r="E123">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="F123">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G123">
+        <v>62.39</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A124" s="2">
+        <v>123</v>
+      </c>
+      <c r="B124">
+        <v>8</v>
+      </c>
+      <c r="C124">
+        <v>58.31</v>
+      </c>
+      <c r="D124">
+        <v>8.92</v>
+      </c>
+      <c r="E124">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="F124">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="G124">
+        <v>66.47</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A125" s="2">
+        <v>124</v>
+      </c>
+      <c r="B125">
+        <v>10</v>
+      </c>
+      <c r="C125">
+        <v>54.89</v>
+      </c>
+      <c r="D125">
+        <v>8.86</v>
+      </c>
+      <c r="E125">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="F125">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G125">
+        <v>62.57</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A126" s="2">
+        <v>125</v>
+      </c>
+      <c r="B126">
+        <v>9</v>
+      </c>
+      <c r="C126">
+        <v>57.27</v>
+      </c>
+      <c r="D126">
+        <v>8.73</v>
+      </c>
+      <c r="E126">
+        <v>0.378</v>
+      </c>
+      <c r="F126">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="G126">
+        <v>65.290000000000006</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A127" s="2">
+        <v>126</v>
+      </c>
+      <c r="B127">
+        <v>8</v>
+      </c>
+      <c r="C127">
+        <v>54.76</v>
+      </c>
+      <c r="D127">
+        <v>8.82</v>
+      </c>
+      <c r="E127">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="F127">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G127">
+        <v>62.43</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A128" s="2">
+        <v>127</v>
+      </c>
+      <c r="B128">
+        <v>11</v>
+      </c>
+      <c r="C128">
+        <v>55.8</v>
+      </c>
+      <c r="D128">
+        <v>10.26</v>
+      </c>
+      <c r="E128">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="F128">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G128">
+        <v>63.61</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A129" s="2">
+        <v>128</v>
+      </c>
+      <c r="B129">
+        <v>10</v>
+      </c>
+      <c r="C129">
+        <v>58.1</v>
+      </c>
+      <c r="D129">
+        <v>9.26</v>
+      </c>
+      <c r="E129">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="F129">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G129">
+        <v>66.23</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A130" s="2">
+        <v>129</v>
+      </c>
+      <c r="B130">
+        <v>10</v>
+      </c>
+      <c r="C130">
+        <v>55.1</v>
+      </c>
+      <c r="D130">
+        <v>9.3800000000000008</v>
+      </c>
+      <c r="E130">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="F130">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G130">
+        <v>62.81</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A131" s="2">
+        <v>130</v>
+      </c>
+      <c r="B131">
+        <v>9</v>
+      </c>
+      <c r="C131">
+        <v>55.4</v>
+      </c>
+      <c r="D131">
+        <v>9.48</v>
+      </c>
+      <c r="E131">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="F131">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G131">
+        <v>63.16</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A132" s="2">
+        <v>131</v>
+      </c>
+      <c r="B132">
+        <v>11</v>
+      </c>
+      <c r="C132">
+        <v>60.9</v>
+      </c>
+      <c r="D132">
+        <v>10.49</v>
+      </c>
+      <c r="E132">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="F132">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G132">
+        <v>69.430000000000007</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A133" s="2">
+        <v>132</v>
+      </c>
+      <c r="B133">
+        <v>9</v>
+      </c>
+      <c r="C133">
+        <v>54.6</v>
+      </c>
+      <c r="D133">
+        <v>9.11</v>
+      </c>
+      <c r="E133">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="F133">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G133">
+        <v>62.25</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A134" s="2">
+        <v>133</v>
+      </c>
+      <c r="B134">
+        <v>10</v>
+      </c>
+      <c r="C134">
+        <v>55.3</v>
+      </c>
+      <c r="D134">
+        <v>9.86</v>
+      </c>
+      <c r="E134">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F134">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G134">
+        <v>63.04</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A135" s="2">
+        <v>134</v>
+      </c>
+      <c r="B135">
+        <v>10</v>
+      </c>
+      <c r="C135">
+        <v>61.1</v>
+      </c>
+      <c r="D135">
+        <v>9.83</v>
+      </c>
+      <c r="E135">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="F135">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G135">
+        <v>69.650000000000006</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A136" s="2">
+        <v>135</v>
+      </c>
+      <c r="B136">
+        <v>8</v>
+      </c>
+      <c r="C136">
+        <v>54.9</v>
+      </c>
+      <c r="D136">
+        <v>10.42</v>
+      </c>
+      <c r="E136">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="F136">
+        <v>0.01</v>
+      </c>
+      <c r="G136">
+        <v>62.59</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A137" s="2">
+        <v>136</v>
+      </c>
+      <c r="B137">
+        <v>10</v>
+      </c>
+      <c r="C137">
+        <v>53.7</v>
+      </c>
+      <c r="D137">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E137">
+        <v>0.505</v>
+      </c>
+      <c r="F137">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G137">
+        <v>61.22</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A138" s="2">
+        <v>137</v>
+      </c>
+      <c r="B138">
+        <v>10</v>
+      </c>
+      <c r="C138">
+        <v>60.9</v>
+      </c>
+      <c r="D138">
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="E138">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="F138">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G138">
+        <v>69.430000000000007</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A139" s="2">
+        <v>138</v>
+      </c>
+      <c r="B139">
+        <v>11</v>
+      </c>
+      <c r="C139">
+        <v>54.1</v>
+      </c>
+      <c r="D139">
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="E139">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="F139">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G139">
+        <v>61.67</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A140" s="2">
+        <v>139</v>
+      </c>
+      <c r="B140">
+        <v>9</v>
+      </c>
+      <c r="C140">
+        <v>55.4</v>
+      </c>
+      <c r="D140">
+        <v>11</v>
+      </c>
+      <c r="E140">
+        <v>0.503</v>
+      </c>
+      <c r="F140">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G140">
+        <v>63.15</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A141" s="2">
+        <v>140</v>
+      </c>
+      <c r="B141">
+        <v>12</v>
+      </c>
+      <c r="C141">
+        <v>54.4</v>
+      </c>
+      <c r="D141">
+        <v>10.47</v>
+      </c>
+      <c r="E141">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F141">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G141">
+        <v>62.01</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A142" s="2">
+        <v>141</v>
+      </c>
+      <c r="B142">
+        <v>12</v>
+      </c>
+      <c r="C142">
+        <v>54.6</v>
+      </c>
+      <c r="D142">
+        <v>10.31</v>
+      </c>
+      <c r="E142">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="F142">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G142">
+        <v>62.24</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A143" s="2">
+        <v>142</v>
+      </c>
+      <c r="B143">
+        <v>10</v>
+      </c>
+      <c r="C143">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="D143">
+        <v>9.89</v>
+      </c>
+      <c r="E143">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="F143">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G143">
+        <v>78.2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A144" s="2">
+        <v>143</v>
+      </c>
+      <c r="B144">
+        <v>8</v>
+      </c>
+      <c r="C144">
+        <v>54.9</v>
+      </c>
+      <c r="D144">
+        <v>10.4</v>
+      </c>
+      <c r="E144">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="F144">
+        <v>0.01</v>
+      </c>
+      <c r="G144">
+        <v>62.59</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A145" s="2">
+        <v>144</v>
+      </c>
+      <c r="B145">
+        <v>9</v>
+      </c>
+      <c r="C145">
+        <v>54.6</v>
+      </c>
+      <c r="D145">
+        <v>10.23</v>
+      </c>
+      <c r="E145">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="F145">
+        <v>0.01</v>
+      </c>
+      <c r="G145">
+        <v>62.24</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A146" s="2">
+        <v>145</v>
+      </c>
+      <c r="B146">
+        <v>13</v>
+      </c>
+      <c r="C146">
+        <v>52.9</v>
+      </c>
+      <c r="D146">
+        <v>10.32</v>
+      </c>
+      <c r="E146">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="F146">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G146">
+        <v>60.3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A147" s="2">
+        <v>146</v>
+      </c>
+      <c r="B147">
+        <v>12</v>
+      </c>
+      <c r="C147">
+        <v>54.2</v>
+      </c>
+      <c r="D147">
+        <v>10.25</v>
+      </c>
+      <c r="E147">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="F147">
+        <v>0.01</v>
+      </c>
+      <c r="G147">
+        <v>61.79</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A148" s="2">
+        <v>147</v>
+      </c>
+      <c r="B148">
+        <v>10</v>
+      </c>
+      <c r="C148">
+        <v>96.57</v>
+      </c>
+      <c r="D148">
+        <v>10.09</v>
+      </c>
+      <c r="E148">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="F148">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G148">
+        <v>110.18</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A149" s="2">
+        <v>148</v>
+      </c>
+      <c r="B149">
+        <v>9</v>
+      </c>
+      <c r="C149">
+        <v>105.06</v>
+      </c>
+      <c r="D149">
+        <v>10.18</v>
+      </c>
+      <c r="E149">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="F149">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G149">
+        <v>119.67</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A150" s="2">
+        <v>149</v>
+      </c>
+      <c r="B150">
+        <v>9</v>
+      </c>
+      <c r="C150">
+        <v>94.73</v>
+      </c>
+      <c r="D150">
+        <v>10.38</v>
+      </c>
+      <c r="E150">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="F150">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G150">
+        <v>107.9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A151" s="2">
+        <v>150</v>
+      </c>
+      <c r="B151">
+        <v>9</v>
+      </c>
+      <c r="C151">
+        <v>106.11</v>
+      </c>
+      <c r="D151">
+        <v>11.06</v>
+      </c>
+      <c r="E151">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="F151">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G151">
+        <v>120.86</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A152" s="2">
+        <v>151</v>
+      </c>
+      <c r="B152">
+        <v>8</v>
+      </c>
+      <c r="C152">
+        <v>93.1</v>
+      </c>
+      <c r="D152">
+        <v>11.02</v>
+      </c>
+      <c r="E152">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="F152">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G152">
+        <v>106.09</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A153" s="2">
+        <v>152</v>
+      </c>
+      <c r="B153">
+        <v>9</v>
+      </c>
+      <c r="C153">
+        <v>107.68</v>
+      </c>
+      <c r="D153">
+        <v>11.02</v>
+      </c>
+      <c r="E153">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="F153">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G153">
+        <v>122.64</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A154" s="2">
+        <v>153</v>
+      </c>
+      <c r="B154">
+        <v>9</v>
+      </c>
+      <c r="C154">
+        <v>97.04</v>
+      </c>
+      <c r="D154">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="E154">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="F154">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G154">
+        <v>110.51</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A155" s="2">
+        <v>154</v>
+      </c>
+      <c r="B155">
+        <v>9</v>
+      </c>
+      <c r="C155">
+        <v>93.28</v>
+      </c>
+      <c r="D155">
+        <v>11.26</v>
+      </c>
+      <c r="E155">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="F155">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G155">
+        <v>106.22</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A156" s="2">
+        <v>155</v>
+      </c>
+      <c r="B156">
+        <v>8</v>
+      </c>
+      <c r="C156">
+        <v>91.03</v>
+      </c>
+      <c r="D156">
+        <v>10.97</v>
+      </c>
+      <c r="E156">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="F156">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G156">
+        <v>103.65</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A157" s="2">
+        <v>156</v>
+      </c>
+      <c r="B157">
+        <v>9</v>
+      </c>
+      <c r="C157">
+        <v>106.02</v>
+      </c>
+      <c r="D157">
+        <v>11.16</v>
+      </c>
+      <c r="E157">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="F157">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G157">
+        <v>120.88</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A158" s="2">
+        <v>157</v>
+      </c>
+      <c r="B158">
+        <v>9</v>
+      </c>
+      <c r="C158">
+        <v>98.19</v>
+      </c>
+      <c r="D158">
+        <v>11.21</v>
+      </c>
+      <c r="E158">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="F158">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G158">
+        <v>111.24</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A159" s="2">
+        <v>158</v>
+      </c>
+      <c r="B159">
+        <v>9</v>
+      </c>
+      <c r="C159">
+        <v>93.67</v>
+      </c>
+      <c r="D159">
+        <v>10.26</v>
+      </c>
+      <c r="E159">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="F159">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G159">
+        <v>106.57</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A160" s="2">
+        <v>159</v>
+      </c>
+      <c r="B160">
+        <v>8</v>
+      </c>
+      <c r="C160">
+        <v>92.8</v>
+      </c>
+      <c r="D160">
+        <v>10.87</v>
+      </c>
+      <c r="E160">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="F160">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G160">
+        <v>105.79</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A161" s="2">
+        <v>160</v>
+      </c>
+      <c r="B161">
+        <v>9</v>
+      </c>
+      <c r="C161">
+        <v>105.85</v>
+      </c>
+      <c r="D161">
+        <v>10.72</v>
+      </c>
+      <c r="E161">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="F161">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G161">
+        <v>120.73</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A162" s="2">
+        <v>161</v>
+      </c>
+      <c r="B162">
+        <v>8</v>
+      </c>
+      <c r="C162">
+        <v>98.09</v>
+      </c>
+      <c r="D162">
+        <v>10.96</v>
+      </c>
+      <c r="E162">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="F162">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G162">
+        <v>111.98</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A163" s="2">
+        <v>162</v>
+      </c>
+      <c r="B163">
+        <v>8</v>
+      </c>
+      <c r="C163">
+        <v>95.28</v>
+      </c>
+      <c r="D163">
+        <v>10.72</v>
+      </c>
+      <c r="E163">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="F163">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G163">
+        <v>108.53</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A164" s="2">
+        <v>163</v>
+      </c>
+      <c r="B164">
+        <v>8</v>
+      </c>
+      <c r="C164">
+        <v>92.55</v>
+      </c>
+      <c r="D164">
+        <v>11.01</v>
+      </c>
+      <c r="E164">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="F164">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G164">
+        <v>105.58</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A165" s="2">
+        <v>164</v>
+      </c>
+      <c r="B165">
+        <v>8</v>
+      </c>
+      <c r="C165">
+        <v>90.78</v>
+      </c>
+      <c r="D165">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="E165">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="F165">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G165">
+        <v>103.7</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A166" s="2">
+        <v>165</v>
+      </c>
+      <c r="B166">
+        <v>9</v>
+      </c>
+      <c r="C166">
+        <v>111.01</v>
+      </c>
+      <c r="D166">
+        <v>11.18</v>
+      </c>
+      <c r="E166">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="F166">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G166">
+        <v>126.55</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A167" s="2">
+        <v>166</v>
+      </c>
+      <c r="B167">
+        <v>8</v>
+      </c>
+      <c r="C167">
+        <v>102.14</v>
+      </c>
+      <c r="D167">
+        <v>11.08</v>
+      </c>
+      <c r="E167">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="F167">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G167">
+        <v>116.48</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A168" s="2">
+        <v>167</v>
+      </c>
+      <c r="B168">
+        <v>8</v>
+      </c>
+      <c r="C168">
+        <v>99.09</v>
+      </c>
+      <c r="D168">
+        <v>11.14</v>
+      </c>
+      <c r="E168">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="F168">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G168">
+        <v>112.9</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A169" s="2">
+        <v>168</v>
+      </c>
+      <c r="B169">
+        <v>8</v>
+      </c>
+      <c r="C169">
+        <v>95.82</v>
+      </c>
+      <c r="D169">
+        <v>10.56</v>
+      </c>
+      <c r="E169">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="F169">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G169">
+        <v>109.33</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A170" s="2">
+        <v>169</v>
+      </c>
+      <c r="B170">
+        <v>8</v>
+      </c>
+      <c r="C170">
+        <v>91.62</v>
+      </c>
+      <c r="D170">
+        <v>10.86</v>
+      </c>
+      <c r="E170">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="F170">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G170">
+        <v>104.48</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A171" s="2">
+        <v>170</v>
+      </c>
+      <c r="B171">
+        <v>8</v>
+      </c>
+      <c r="C171">
+        <v>90.38</v>
+      </c>
+      <c r="D171">
+        <v>10.61</v>
+      </c>
+      <c r="E171">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="F171">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G171">
+        <v>103.05</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A172" s="2">
+        <v>171</v>
+      </c>
+      <c r="B172">
+        <v>8</v>
+      </c>
+      <c r="C172">
+        <v>112.15</v>
+      </c>
+      <c r="D172">
+        <v>10.85</v>
+      </c>
+      <c r="E172">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="F172">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G172">
+        <v>127.75</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A173" s="2">
+        <v>172</v>
+      </c>
+      <c r="B173">
+        <v>8</v>
+      </c>
+      <c r="C173">
+        <v>101.08</v>
+      </c>
+      <c r="D173">
+        <v>10.9</v>
+      </c>
+      <c r="E173">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="F173">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G173">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A174" s="2">
+        <v>173</v>
+      </c>
+      <c r="B174">
+        <v>8</v>
+      </c>
+      <c r="C174">
+        <v>96.36</v>
+      </c>
+      <c r="D174">
+        <v>10.79</v>
+      </c>
+      <c r="E174">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="F174">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G174">
+        <v>109.8</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A175" s="2">
+        <v>174</v>
+      </c>
+      <c r="B175">
+        <v>8</v>
+      </c>
+      <c r="C175">
+        <v>93.35</v>
+      </c>
+      <c r="D175">
+        <v>10.95</v>
+      </c>
+      <c r="E175">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="F175">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G175">
+        <v>106.4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A176" s="2">
+        <v>175</v>
+      </c>
+      <c r="B176">
+        <v>8</v>
+      </c>
+      <c r="C176">
+        <v>91.61</v>
+      </c>
+      <c r="D176">
+        <v>10.99</v>
+      </c>
+      <c r="E176">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="F176">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G176">
+        <v>104.48</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A177" s="2">
+        <v>176</v>
+      </c>
+      <c r="B177">
+        <v>9</v>
+      </c>
+      <c r="C177">
+        <v>90.55</v>
+      </c>
+      <c r="D177">
+        <v>11.01</v>
+      </c>
+      <c r="E177">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="F177">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G177">
+        <v>103.42</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A178" s="2">
+        <v>177</v>
+      </c>
+      <c r="B178">
+        <v>10</v>
+      </c>
+      <c r="C178">
+        <v>58.3</v>
+      </c>
+      <c r="D178">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="E178">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="F178">
+        <v>0.01</v>
+      </c>
+      <c r="G178">
+        <v>66.459999999999994</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A179" s="2">
+        <v>178</v>
+      </c>
+      <c r="B179">
+        <v>9</v>
+      </c>
+      <c r="C179">
+        <v>57.4</v>
+      </c>
+      <c r="D179">
+        <v>11.2</v>
+      </c>
+      <c r="E179">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="F179">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G179">
+        <v>65.44</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A180" s="2">
+        <v>179</v>
+      </c>
+      <c r="B180">
+        <v>9</v>
+      </c>
+      <c r="C180">
+        <v>54.7</v>
+      </c>
+      <c r="D180">
+        <v>10</v>
+      </c>
+      <c r="E180">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="F180">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G180">
+        <v>62.36</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A181" s="2">
+        <v>180</v>
+      </c>
+      <c r="B181">
+        <v>9</v>
+      </c>
+      <c r="C181">
+        <v>55.4</v>
+      </c>
+      <c r="D181">
+        <v>10.7</v>
+      </c>
+      <c r="E181">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="F181">
+        <v>0.01</v>
+      </c>
+      <c r="G181">
+        <v>63.15</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A182" s="2">
+        <v>181</v>
+      </c>
+      <c r="B182">
+        <v>9</v>
+      </c>
+      <c r="C182">
+        <v>58.7</v>
+      </c>
+      <c r="D182">
+        <v>11.1</v>
+      </c>
+      <c r="E182">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="F182">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G182">
+        <v>66.92</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A183" s="2">
+        <v>182</v>
+      </c>
+      <c r="B183">
+        <v>9</v>
+      </c>
+      <c r="C183">
+        <v>54.3</v>
+      </c>
+      <c r="D183">
+        <v>10</v>
+      </c>
+      <c r="E183">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="F183">
+        <v>0.01</v>
+      </c>
+      <c r="G183">
+        <v>61.9</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A184" s="2">
+        <v>183</v>
+      </c>
+      <c r="B184">
+        <v>10</v>
+      </c>
+      <c r="C184">
+        <v>60.2</v>
+      </c>
+      <c r="D184">
+        <v>11.1</v>
+      </c>
+      <c r="E184">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="F184">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G184">
+        <v>68.63</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A185" s="2">
+        <v>184</v>
+      </c>
+      <c r="B185">
+        <v>9</v>
+      </c>
+      <c r="C185">
+        <v>54.8</v>
+      </c>
+      <c r="D185">
+        <v>9.6</v>
+      </c>
+      <c r="E185">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="F185">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G185">
+        <v>62.47</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A186" s="2">
+        <v>185</v>
+      </c>
+      <c r="B186">
+        <v>9</v>
+      </c>
+      <c r="C186">
+        <v>54.9</v>
+      </c>
+      <c r="D186">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E186">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="F186">
+        <v>0.01</v>
+      </c>
+      <c r="G186">
+        <v>62.59</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A187" s="2">
+        <v>186</v>
+      </c>
+      <c r="B187">
+        <v>10</v>
+      </c>
+      <c r="C187">
+        <v>58.3</v>
+      </c>
+      <c r="D187">
+        <v>11.1</v>
+      </c>
+      <c r="E187">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="F187">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G187">
+        <v>66.459999999999994</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A188" s="2">
+        <v>187</v>
+      </c>
+      <c r="B188">
+        <v>9</v>
+      </c>
+      <c r="C188">
+        <v>54.8</v>
+      </c>
+      <c r="D188">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="E188">
+        <v>0.439</v>
+      </c>
+      <c r="F188">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G188">
+        <v>62.47</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A189" s="2">
+        <v>188</v>
+      </c>
+      <c r="B189">
+        <v>9</v>
+      </c>
+      <c r="C189">
+        <v>60.6</v>
+      </c>
+      <c r="D189">
+        <v>10.4</v>
+      </c>
+      <c r="E189">
+        <v>0.45</v>
+      </c>
+      <c r="F189">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G189">
+        <v>69.08</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A190" s="2">
+        <v>189</v>
+      </c>
+      <c r="B190">
+        <v>9</v>
+      </c>
+      <c r="C190">
+        <v>54.5</v>
+      </c>
+      <c r="D190">
+        <v>10.5</v>
+      </c>
+      <c r="E190">
+        <v>0.436</v>
+      </c>
+      <c r="F190">
+        <v>0.01</v>
+      </c>
+      <c r="G190">
+        <v>62.13</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A191" s="2">
+        <v>190</v>
+      </c>
+      <c r="B191">
+        <v>9</v>
+      </c>
+      <c r="C191">
+        <v>54.8</v>
+      </c>
+      <c r="D191">
+        <v>11.2</v>
+      </c>
+      <c r="E191">
+        <v>0.435</v>
+      </c>
+      <c r="F191">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G191">
+        <v>62.47</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A192" s="2">
+        <v>191</v>
+      </c>
+      <c r="B192">
+        <v>10</v>
+      </c>
+      <c r="C192">
+        <v>58</v>
+      </c>
+      <c r="D192">
+        <v>10.7</v>
+      </c>
+      <c r="E192">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="F192">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G192">
+        <v>66.12</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A193" s="2">
+        <v>192</v>
+      </c>
+      <c r="B193">
+        <v>9</v>
+      </c>
+      <c r="C193">
+        <v>54.9</v>
+      </c>
+      <c r="D193">
+        <v>10.6</v>
+      </c>
+      <c r="E193">
+        <v>0.43</v>
+      </c>
+      <c r="F193">
+        <v>0.01</v>
+      </c>
+      <c r="G193">
+        <v>62.59</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A194" s="2">
+        <v>193</v>
+      </c>
+      <c r="B194">
+        <v>9</v>
+      </c>
+      <c r="C194">
+        <v>54.5</v>
+      </c>
+      <c r="D194">
+        <v>10.7</v>
+      </c>
+      <c r="E194">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="F194">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G194">
+        <v>62.13</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A195" s="2">
+        <v>194</v>
+      </c>
+      <c r="B195">
+        <v>10</v>
+      </c>
+      <c r="C195">
+        <v>58.1</v>
+      </c>
+      <c r="D195">
+        <v>10.1</v>
+      </c>
+      <c r="E195">
+        <v>0.47</v>
+      </c>
+      <c r="F195">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G195">
+        <v>66.23</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A196" s="2">
+        <v>195</v>
+      </c>
+      <c r="B196">
+        <v>9</v>
+      </c>
+      <c r="C196">
+        <v>54.6</v>
+      </c>
+      <c r="D196">
+        <v>10.5</v>
+      </c>
+      <c r="E196">
+        <v>0.432</v>
+      </c>
+      <c r="F196">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G196">
+        <v>62.24</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A197" s="2">
+        <v>196</v>
+      </c>
+      <c r="B197">
+        <v>10</v>
+      </c>
+      <c r="C197">
+        <v>54.8</v>
+      </c>
+      <c r="D197">
+        <v>10.9</v>
+      </c>
+      <c r="E197">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="F197">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G197">
+        <v>62.47</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A198" s="2">
+        <v>197</v>
+      </c>
+      <c r="B198">
+        <v>10</v>
+      </c>
+      <c r="C198">
+        <v>58</v>
+      </c>
+      <c r="D198">
+        <v>11</v>
+      </c>
+      <c r="E198">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="F198">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G198">
+        <v>66.12</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A199" s="2">
+        <v>198</v>
+      </c>
+      <c r="B199">
+        <v>10</v>
+      </c>
+      <c r="C199">
+        <v>54.9</v>
+      </c>
+      <c r="D199">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E199">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="F199">
+        <v>0.01</v>
+      </c>
+      <c r="G199">
+        <v>62.59</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A200" s="2">
+        <v>199</v>
+      </c>
+      <c r="B200">
+        <v>9</v>
+      </c>
+      <c r="C200">
+        <v>54.8</v>
+      </c>
+      <c r="D200">
+        <v>10.8</v>
+      </c>
+      <c r="E200">
+        <v>0.432</v>
+      </c>
+      <c r="F200">
+        <v>0.01</v>
+      </c>
+      <c r="G200">
+        <v>62.47</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A201" s="2">
+        <v>200</v>
+      </c>
+      <c r="B201">
+        <v>10</v>
+      </c>
+      <c r="C201">
+        <v>58.1</v>
+      </c>
+      <c r="D201">
+        <v>10.9</v>
+      </c>
+      <c r="E201">
+        <v>0.46</v>
+      </c>
+      <c r="F201">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G201">
+        <v>66.23</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A202" s="2">
+        <v>201</v>
+      </c>
+      <c r="B202">
+        <v>9</v>
+      </c>
+      <c r="C202">
+        <v>54.9</v>
+      </c>
+      <c r="D202">
+        <v>10.7</v>
+      </c>
+      <c r="E202">
+        <v>0.432</v>
+      </c>
+      <c r="F202">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G202">
+        <v>62.59</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A203" s="2">
+        <v>202</v>
+      </c>
+      <c r="B203">
+        <v>9</v>
+      </c>
+      <c r="C203">
+        <v>55.1</v>
+      </c>
+      <c r="D203">
+        <v>10.8</v>
+      </c>
+      <c r="E203">
+        <v>0.438</v>
+      </c>
+      <c r="F203">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G203">
+        <v>62.81</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A204" s="2">
+        <v>203</v>
+      </c>
+      <c r="B204">
+        <v>10</v>
+      </c>
+      <c r="C204">
+        <v>58.5</v>
+      </c>
+      <c r="D204">
+        <v>10.7</v>
+      </c>
+      <c r="E204">
+        <v>0.47</v>
+      </c>
+      <c r="F204">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G204">
+        <v>66.69</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A205" s="2">
+        <v>204</v>
+      </c>
+      <c r="B205">
+        <v>9</v>
+      </c>
+      <c r="C205">
+        <v>55.1</v>
+      </c>
+      <c r="D205">
+        <v>11.1</v>
+      </c>
+      <c r="E205">
+        <v>0.432</v>
+      </c>
+      <c r="F205">
+        <v>0.01</v>
+      </c>
+      <c r="G205">
+        <v>62.81</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A206" s="2">
+        <v>205</v>
+      </c>
+      <c r="B206">
+        <v>9</v>
+      </c>
+      <c r="C206">
+        <v>54.8</v>
+      </c>
+      <c r="D206">
+        <v>11.2</v>
+      </c>
+      <c r="E206">
+        <v>0.438</v>
+      </c>
+      <c r="F206">
+        <v>0.01</v>
+      </c>
+      <c r="G206">
+        <v>62.47</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A207" s="2">
+        <v>206</v>
+      </c>
+      <c r="B207">
+        <v>10</v>
+      </c>
+      <c r="C207">
+        <v>58.2</v>
+      </c>
+      <c r="D207">
+        <v>10.8</v>
+      </c>
+      <c r="E207">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="F207">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G207">
+        <v>66.349999999999994</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A208" s="2">
+        <v>207</v>
+      </c>
+      <c r="B208">
+        <v>9</v>
+      </c>
+      <c r="C208">
+        <v>107.31</v>
+      </c>
+      <c r="D208">
+        <v>11.03</v>
+      </c>
+      <c r="E208">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="F208">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G208">
+        <v>122.24</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A209" s="2">
+        <v>208</v>
+      </c>
+      <c r="B209">
+        <v>9</v>
+      </c>
+      <c r="C209">
+        <v>99.72</v>
+      </c>
+      <c r="D209">
+        <v>10.38</v>
+      </c>
+      <c r="E209">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="F209">
+        <v>2E-3</v>
+      </c>
+      <c r="G209">
+        <v>113.69</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A210" s="2">
+        <v>209</v>
+      </c>
+      <c r="B210">
+        <v>9</v>
+      </c>
+      <c r="C210">
+        <v>113.86</v>
+      </c>
+      <c r="D210">
+        <v>10.74</v>
+      </c>
+      <c r="E210">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="F210">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G210">
+        <v>129.71</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A211" s="2">
+        <v>210</v>
+      </c>
+      <c r="B211">
+        <v>9</v>
+      </c>
+      <c r="C211">
+        <v>108.45</v>
+      </c>
+      <c r="D211">
+        <v>10.39</v>
+      </c>
+      <c r="E211">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="F211">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G211">
+        <v>123.55</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A212" s="2">
+        <v>211</v>
+      </c>
+      <c r="B212">
+        <v>9</v>
+      </c>
+      <c r="C212">
+        <v>102.29</v>
+      </c>
+      <c r="D212">
+        <v>10.39</v>
+      </c>
+      <c r="E212">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="F212">
+        <v>2E-3</v>
+      </c>
+      <c r="G212">
+        <v>116.64</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A213" s="2">
+        <v>212</v>
+      </c>
+      <c r="B213">
+        <v>9</v>
+      </c>
+      <c r="C213">
+        <v>116.87</v>
+      </c>
+      <c r="D213">
+        <v>11.06</v>
+      </c>
+      <c r="E213">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="F213">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G213">
+        <v>133.19</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A214" s="2">
+        <v>213</v>
+      </c>
+      <c r="B214">
+        <v>9</v>
+      </c>
+      <c r="C214">
+        <v>100.88</v>
+      </c>
+      <c r="D214">
+        <v>10.67</v>
+      </c>
+      <c r="E214">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="F214">
+        <v>2E-3</v>
+      </c>
+      <c r="G214">
+        <v>115.01</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A215" s="2">
+        <v>214</v>
+      </c>
+      <c r="B215">
+        <v>9</v>
+      </c>
+      <c r="C215">
+        <v>114.06</v>
+      </c>
+      <c r="D215">
+        <v>11.01</v>
+      </c>
+      <c r="E215">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="F215">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G215">
+        <v>130.03</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A216" s="2">
+        <v>215</v>
+      </c>
+      <c r="B216">
+        <v>9</v>
+      </c>
+      <c r="C216">
+        <v>98.66</v>
+      </c>
+      <c r="D216">
+        <v>10.53</v>
+      </c>
+      <c r="E216">
+        <v>0.314</v>
+      </c>
+      <c r="F216">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G216">
+        <v>112.38</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A217" s="2">
+        <v>216</v>
+      </c>
+      <c r="B217">
+        <v>9</v>
+      </c>
+      <c r="C217">
+        <v>114.03</v>
+      </c>
+      <c r="D217">
+        <v>11.05</v>
+      </c>
+      <c r="E217">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="F217">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G217">
+        <v>129.99</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A218" s="2">
+        <v>217</v>
+      </c>
+      <c r="B218">
+        <v>9</v>
+      </c>
+      <c r="C218">
+        <v>100.88</v>
+      </c>
+      <c r="D218">
+        <v>10.09</v>
+      </c>
+      <c r="E218">
+        <v>0.312</v>
+      </c>
+      <c r="F218">
+        <v>2E-3</v>
+      </c>
+      <c r="G218">
+        <v>114.99</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A219" s="2">
+        <v>218</v>
+      </c>
+      <c r="B219">
+        <v>9</v>
+      </c>
+      <c r="C219">
+        <v>109.52</v>
+      </c>
+      <c r="D219">
+        <v>10.99</v>
+      </c>
+      <c r="E219">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="F219">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G219">
+        <v>124.9</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A220" s="2">
+        <v>219</v>
+      </c>
+      <c r="B220">
+        <v>9</v>
+      </c>
+      <c r="C220">
+        <v>98.88</v>
+      </c>
+      <c r="D220">
+        <v>10.8</v>
+      </c>
+      <c r="E220">
+        <v>0.33</v>
+      </c>
+      <c r="F220">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G220">
+        <v>112.74</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A221" s="2">
+        <v>220</v>
+      </c>
+      <c r="B221">
+        <v>9</v>
+      </c>
+      <c r="C221">
+        <v>110.55</v>
+      </c>
+      <c r="D221">
+        <v>11.18</v>
+      </c>
+      <c r="E221">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="F221">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G221">
+        <v>125.83</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A222" s="2">
+        <v>221</v>
+      </c>
+      <c r="B222">
+        <v>9</v>
+      </c>
+      <c r="C222">
+        <v>98.11</v>
+      </c>
+      <c r="D222">
+        <v>9.83</v>
+      </c>
+      <c r="E222">
+        <v>0.307</v>
+      </c>
+      <c r="F222">
+        <v>2E-3</v>
+      </c>
+      <c r="G222">
+        <v>111.85</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A223" s="2">
+        <v>222</v>
+      </c>
+      <c r="B223">
+        <v>9</v>
+      </c>
+      <c r="C223">
+        <v>116.58</v>
+      </c>
+      <c r="D223">
+        <v>11.02</v>
+      </c>
+      <c r="E223">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="F223">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G223">
+        <v>132.86000000000001</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A224" s="2">
+        <v>223</v>
+      </c>
+      <c r="B224">
+        <v>9</v>
+      </c>
+      <c r="C224">
+        <v>99.66</v>
+      </c>
+      <c r="D224">
+        <v>10.49</v>
+      </c>
+      <c r="E224">
+        <v>0.307</v>
+      </c>
+      <c r="F224">
+        <v>2E-3</v>
+      </c>
+      <c r="G224">
+        <v>113.64</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A225" s="2">
+        <v>224</v>
+      </c>
+      <c r="B225">
+        <v>9</v>
+      </c>
+      <c r="C225">
+        <v>103.55</v>
+      </c>
+      <c r="D225">
+        <v>10.78</v>
+      </c>
+      <c r="E225">
+        <v>0.318</v>
+      </c>
+      <c r="F225">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="G225">
+        <v>118.08</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A226" s="2">
+        <v>225</v>
+      </c>
+      <c r="B226">
+        <v>9</v>
+      </c>
+      <c r="C226">
+        <v>99.01</v>
+      </c>
+      <c r="D226">
+        <v>10.67</v>
+      </c>
+      <c r="E226">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="F226">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G226">
+        <v>112.88</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A227" s="2">
+        <v>226</v>
+      </c>
+      <c r="B227">
+        <v>9</v>
+      </c>
+      <c r="C227">
+        <v>106</v>
+      </c>
+      <c r="D227">
+        <v>10.84</v>
+      </c>
+      <c r="E227">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="F227">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G227">
+        <v>120.84</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A228" s="2">
+        <v>227</v>
+      </c>
+      <c r="B228">
+        <v>9</v>
+      </c>
+      <c r="C228">
+        <v>98.44</v>
+      </c>
+      <c r="D228">
+        <v>10.34</v>
+      </c>
+      <c r="E228">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="F228">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G228">
+        <v>112.18</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A229" s="2">
+        <v>228</v>
+      </c>
+      <c r="B229">
+        <v>9</v>
+      </c>
+      <c r="C229">
+        <v>99.88</v>
+      </c>
+      <c r="D229">
+        <v>10.23</v>
+      </c>
+      <c r="E229">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="F229">
+        <v>2E-3</v>
+      </c>
+      <c r="G229">
+        <v>113.86</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A230" s="2">
+        <v>229</v>
+      </c>
+      <c r="B230">
+        <v>9</v>
+      </c>
+      <c r="C230">
+        <v>99.11</v>
+      </c>
+      <c r="D230">
+        <v>10.45</v>
+      </c>
+      <c r="E230">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="F230">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G230">
+        <v>112.96</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A231" s="2">
+        <v>230</v>
+      </c>
+      <c r="B231">
+        <v>9</v>
+      </c>
+      <c r="C231">
+        <v>112.88</v>
+      </c>
+      <c r="D231">
+        <v>11.04</v>
+      </c>
+      <c r="E231">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="F231">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G231">
+        <v>128.6</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A232" s="2">
+        <v>231</v>
+      </c>
+      <c r="B232">
+        <v>9</v>
+      </c>
+      <c r="C232">
+        <v>99</v>
+      </c>
+      <c r="D232">
+        <v>10.4</v>
+      </c>
+      <c r="E232">
+        <v>0.307</v>
+      </c>
+      <c r="F232">
+        <v>2E-3</v>
+      </c>
+      <c r="G232">
+        <v>112.86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>